<commit_message>
feat: adiciona a interface grafica e algumas melhorias extras
</commit_message>
<xml_diff>
--- a/data/RPONTES.xlsx
+++ b/data/RPONTES.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DanielyVasconcelos\Documents\Projetos-Portifolio\gerador-documentos\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65FBD27F-1D61-47BB-AEE2-6AD25D309B58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE9502A0-DE74-4BFC-A8A4-FCAF14551F31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="256">
   <si>
     <t>ID_Proposta</t>
   </si>
@@ -772,6 +772,30 @@
   </si>
   <si>
     <t>032/2025</t>
+  </si>
+  <si>
+    <t>033/2025</t>
+  </si>
+  <si>
+    <t>Daniely Evellin</t>
+  </si>
+  <si>
+    <t>456.789.123-55</t>
+  </si>
+  <si>
+    <t>dani.evellin@email.com</t>
+  </si>
+  <si>
+    <t>034/2025</t>
+  </si>
+  <si>
+    <t>123.456.789-55</t>
+  </si>
+  <si>
+    <t>Erika Polina</t>
+  </si>
+  <si>
+    <t>erika.poliana@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -1059,10 +1083,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1072,7 +1096,7 @@
     <col min="4" max="4" width="22.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1089,7 +1113,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -1106,7 +1130,7 @@
         <v>45672</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -1123,7 +1147,7 @@
         <v>45708</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -1140,7 +1164,7 @@
         <v>45726</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -1157,7 +1181,7 @@
         <v>45752</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>21</v>
       </c>
@@ -1174,7 +1198,7 @@
         <v>45795</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>25</v>
       </c>
@@ -1191,7 +1215,7 @@
         <v>45830</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>29</v>
       </c>
@@ -1208,7 +1232,7 @@
         <v>45839</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>33</v>
       </c>
@@ -1225,7 +1249,7 @@
         <v>45883</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>37</v>
       </c>
@@ -1242,7 +1266,7 @@
         <v>45909</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>41</v>
       </c>
@@ -1259,7 +1283,7 @@
         <v>45955</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>45</v>
       </c>
@@ -1276,7 +1300,7 @@
         <v>45991</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>49</v>
       </c>
@@ -1293,7 +1317,7 @@
         <v>46003</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>53</v>
       </c>
@@ -1310,7 +1334,7 @@
         <v>46027</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>57</v>
       </c>
@@ -1327,7 +1351,7 @@
         <v>46081</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>61</v>
       </c>
@@ -1344,7 +1368,7 @@
         <v>46096</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>65</v>
       </c>
@@ -1361,7 +1385,7 @@
         <v>46113</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>69</v>
       </c>
@@ -1378,7 +1402,7 @@
         <v>46162</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>73</v>
       </c>
@@ -1395,7 +1419,7 @@
         <v>46198</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>77</v>
       </c>
@@ -1412,7 +1436,7 @@
         <v>46214</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>81</v>
       </c>
@@ -1429,7 +1453,7 @@
         <v>46242</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>85</v>
       </c>
@@ -1446,7 +1470,7 @@
         <v>46282</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>89</v>
       </c>
@@ -1463,7 +1487,7 @@
         <v>46297</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>93</v>
       </c>
@@ -1480,7 +1504,7 @@
         <v>46335</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>97</v>
       </c>
@@ -1497,7 +1521,7 @@
         <v>46360</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>101</v>
       </c>
@@ -1514,7 +1538,7 @@
         <v>46408</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>105</v>
       </c>
@@ -1531,7 +1555,7 @@
         <v>46432</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>109</v>
       </c>
@@ -1548,7 +1572,7 @@
         <v>46475</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>113</v>
       </c>
@@ -1565,7 +1589,7 @@
         <v>46489</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>117</v>
       </c>
@@ -1582,7 +1606,7 @@
         <v>46514</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>121</v>
       </c>
@@ -1630,6 +1654,40 @@
         <v>246</v>
       </c>
       <c r="E33" s="7">
+        <v>45927</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="E34" s="7">
+        <v>45927</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>255</v>
+      </c>
+      <c r="E35" s="7">
         <v>45927</v>
       </c>
     </row>
@@ -1637,6 +1695,8 @@
   <hyperlinks>
     <hyperlink ref="D32" r:id="rId1" xr:uid="{084DC1CC-A1CE-4FC3-9FDD-9900C3344F5C}"/>
     <hyperlink ref="D33" r:id="rId2" xr:uid="{99642E6B-415B-4623-A258-B9B7121BF997}"/>
+    <hyperlink ref="D34" r:id="rId3" xr:uid="{A58EF8E8-156B-42C9-91D8-90A2D0B3AED7}"/>
+    <hyperlink ref="D35" r:id="rId4" xr:uid="{0E8C2316-32F5-442B-90E6-C0C9350BD5E8}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -1647,10 +1707,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A33" sqref="A33:D33"/>
+      <selection activeCell="A35" sqref="A35:D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1660,7 +1720,7 @@
     <col min="5" max="5" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>125</v>
       </c>
@@ -1676,7 +1736,7 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>129</v>
       </c>
@@ -1692,7 +1752,7 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>133</v>
       </c>
@@ -1708,7 +1768,7 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>137</v>
       </c>
@@ -1724,7 +1784,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>141</v>
       </c>
@@ -1740,7 +1800,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>145</v>
       </c>
@@ -1756,7 +1816,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>148</v>
       </c>
@@ -1772,7 +1832,7 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>152</v>
       </c>
@@ -1788,7 +1848,7 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>155</v>
       </c>
@@ -1804,7 +1864,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>158</v>
       </c>
@@ -1820,7 +1880,7 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>161</v>
       </c>
@@ -1836,7 +1896,7 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>164</v>
       </c>
@@ -1852,7 +1912,7 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>167</v>
       </c>
@@ -1868,7 +1928,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>170</v>
       </c>
@@ -1884,7 +1944,7 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>173</v>
       </c>
@@ -1900,7 +1960,7 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>176</v>
       </c>
@@ -1916,7 +1976,7 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>179</v>
       </c>
@@ -1932,7 +1992,7 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>182</v>
       </c>
@@ -1948,7 +2008,7 @@
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>185</v>
       </c>
@@ -1964,7 +2024,7 @@
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>188</v>
       </c>
@@ -1980,7 +2040,7 @@
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>191</v>
       </c>
@@ -1996,7 +2056,7 @@
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>194</v>
       </c>
@@ -2012,7 +2072,7 @@
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>197</v>
       </c>
@@ -2028,7 +2088,7 @@
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>200</v>
       </c>
@@ -2044,7 +2104,7 @@
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>203</v>
       </c>
@@ -2060,7 +2120,7 @@
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>206</v>
       </c>
@@ -2076,7 +2136,7 @@
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>209</v>
       </c>
@@ -2092,7 +2152,7 @@
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>212</v>
       </c>
@@ -2108,7 +2168,7 @@
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>215</v>
       </c>
@@ -2124,7 +2184,7 @@
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>218</v>
       </c>
@@ -2140,7 +2200,7 @@
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>221</v>
       </c>
@@ -2181,6 +2241,34 @@
         <v>222</v>
       </c>
       <c r="D33" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="D35" s="1" t="s">
         <v>223</v>
       </c>
     </row>
@@ -2194,10 +2282,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A33" sqref="A33:D33"/>
+      <selection activeCell="A35" sqref="A35:D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2206,7 +2294,7 @@
     <col min="4" max="4" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>224</v>
       </c>
@@ -2220,7 +2308,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>350000</v>
       </c>
@@ -2234,7 +2322,7 @@
         <v>45448</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <v>420000</v>
       </c>
@@ -2248,7 +2336,7 @@
         <v>45483</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>510000</v>
       </c>
@@ -2262,7 +2350,7 @@
         <v>45519</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>280000</v>
       </c>
@@ -2276,7 +2364,7 @@
         <v>45555</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>330000</v>
       </c>
@@ -2290,7 +2378,7 @@
         <v>45590</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>650000</v>
       </c>
@@ -2304,7 +2392,7 @@
         <v>45626</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <v>390000</v>
       </c>
@@ -2318,7 +2406,7 @@
         <v>45631</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
         <v>295000</v>
       </c>
@@ -2332,7 +2420,7 @@
         <v>45667</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <v>590000</v>
       </c>
@@ -2346,7 +2434,7 @@
         <v>45703</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
         <v>470000</v>
       </c>
@@ -2360,7 +2448,7 @@
         <v>45736</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
         <v>340000</v>
       </c>
@@ -2374,7 +2462,7 @@
         <v>45772</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
         <v>305000</v>
       </c>
@@ -2388,7 +2476,7 @@
         <v>45807</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
         <v>455000</v>
       </c>
@@ -2402,7 +2490,7 @@
         <v>45813</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
         <v>620000</v>
       </c>
@@ -2416,7 +2504,7 @@
         <v>45848</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
         <v>380000</v>
       </c>
@@ -2430,7 +2518,7 @@
         <v>45884</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
         <v>275000</v>
       </c>
@@ -2444,7 +2532,7 @@
         <v>45920</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
         <v>410000</v>
       </c>
@@ -2458,7 +2546,7 @@
         <v>45955</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="4">
         <v>680000</v>
       </c>
@@ -2472,7 +2560,7 @@
         <v>45991</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
         <v>395000</v>
       </c>
@@ -2486,7 +2574,7 @@
         <v>45996</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
         <v>320000</v>
       </c>
@@ -2500,7 +2588,7 @@
         <v>46032</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="4">
         <v>460000</v>
       </c>
@@ -2514,7 +2602,7 @@
         <v>46068</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="4">
         <v>365000</v>
       </c>
@@ -2528,7 +2616,7 @@
         <v>46101</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="4">
         <v>540000</v>
       </c>
@@ -2542,7 +2630,7 @@
         <v>46137</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="4">
         <v>700000</v>
       </c>
@@ -2556,7 +2644,7 @@
         <v>46172</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="4">
         <v>315000</v>
       </c>
@@ -2570,7 +2658,7 @@
         <v>46178</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="4">
         <v>485000</v>
       </c>
@@ -2584,7 +2672,7 @@
         <v>46213</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="4">
         <v>375000</v>
       </c>
@@ -2598,7 +2686,7 @@
         <v>46249</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="4">
         <v>555000</v>
       </c>
@@ -2612,7 +2700,7 @@
         <v>46285</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="4">
         <v>430000</v>
       </c>
@@ -2626,7 +2714,7 @@
         <v>46320</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="4">
         <v>300000</v>
       </c>
@@ -2665,6 +2753,34 @@
         <v>30</v>
       </c>
       <c r="D33" s="3">
+        <v>46356</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="4">
+        <v>300000</v>
+      </c>
+      <c r="B34" s="4">
+        <v>60000</v>
+      </c>
+      <c r="C34" s="5">
+        <v>30</v>
+      </c>
+      <c r="D34" s="3">
+        <v>46356</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="4">
+        <v>300000</v>
+      </c>
+      <c r="B35" s="4">
+        <v>60000</v>
+      </c>
+      <c r="C35" s="5">
+        <v>30</v>
+      </c>
+      <c r="D35" s="3">
         <v>46356</v>
       </c>
     </row>
@@ -2678,10 +2794,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A33" sqref="A33:B33"/>
+      <selection activeCell="A35" sqref="A35:B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2690,7 +2806,7 @@
     <col min="2" max="2" width="34.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>228</v>
       </c>
@@ -2700,7 +2816,7 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>230</v>
       </c>
@@ -2710,7 +2826,7 @@
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>230</v>
       </c>
@@ -2720,7 +2836,7 @@
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>232</v>
       </c>
@@ -2730,7 +2846,7 @@
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>230</v>
       </c>
@@ -2740,7 +2856,7 @@
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>230</v>
       </c>
@@ -2750,7 +2866,7 @@
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>232</v>
       </c>
@@ -2760,7 +2876,7 @@
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>230</v>
       </c>
@@ -2770,7 +2886,7 @@
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>230</v>
       </c>
@@ -2780,7 +2896,7 @@
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>230</v>
       </c>
@@ -2790,7 +2906,7 @@
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>232</v>
       </c>
@@ -2800,7 +2916,7 @@
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>230</v>
       </c>
@@ -2810,7 +2926,7 @@
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>230</v>
       </c>
@@ -2820,7 +2936,7 @@
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>230</v>
       </c>
@@ -2830,7 +2946,7 @@
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>230</v>
       </c>
@@ -2840,7 +2956,7 @@
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>232</v>
       </c>
@@ -2850,7 +2966,7 @@
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>230</v>
       </c>
@@ -2860,7 +2976,7 @@
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>230</v>
       </c>
@@ -2870,7 +2986,7 @@
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>230</v>
       </c>
@@ -2880,7 +2996,7 @@
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>232</v>
       </c>
@@ -2890,7 +3006,7 @@
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>230</v>
       </c>
@@ -2900,7 +3016,7 @@
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>230</v>
       </c>
@@ -2910,7 +3026,7 @@
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>230</v>
       </c>
@@ -2920,7 +3036,7 @@
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>230</v>
       </c>
@@ -2930,7 +3046,7 @@
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>232</v>
       </c>
@@ -2940,7 +3056,7 @@
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>230</v>
       </c>
@@ -2950,7 +3066,7 @@
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>230</v>
       </c>
@@ -2960,7 +3076,7 @@
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>230</v>
       </c>
@@ -2970,7 +3086,7 @@
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>232</v>
       </c>
@@ -2980,7 +3096,7 @@
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>230</v>
       </c>
@@ -2990,7 +3106,7 @@
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>230</v>
       </c>
@@ -3013,6 +3129,22 @@
         <v>230</v>
       </c>
       <c r="B33" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>231</v>
       </c>
     </row>

</xml_diff>